<commit_message>
peoduct name adjuste din dataset
</commit_message>
<xml_diff>
--- a/data/demand_prediction_weekly.xlsx
+++ b/data/demand_prediction_weekly.xlsx
@@ -463,7 +463,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -484,7 +484,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -505,7 +505,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -526,7 +526,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
@@ -547,7 +547,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
@@ -568,7 +568,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
@@ -589,7 +589,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -610,7 +610,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -631,7 +631,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -652,7 +652,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -673,7 +673,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -694,7 +694,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -715,7 +715,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -736,7 +736,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
@@ -757,7 +757,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
@@ -778,7 +778,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -799,7 +799,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
@@ -820,7 +820,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
@@ -841,7 +841,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
@@ -862,7 +862,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
@@ -883,7 +883,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
@@ -904,7 +904,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -925,7 +925,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -946,7 +946,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -967,7 +967,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -988,7 +988,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1009,7 +1009,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
@@ -1030,7 +1030,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
@@ -1051,7 +1051,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -1072,7 +1072,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -1093,7 +1093,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -1114,7 +1114,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
@@ -1135,7 +1135,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
@@ -1156,7 +1156,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -1177,7 +1177,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
@@ -1198,7 +1198,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
@@ -1219,7 +1219,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
@@ -1240,7 +1240,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
@@ -1261,7 +1261,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
@@ -1282,7 +1282,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1303,7 +1303,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1324,7 +1324,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -1345,7 +1345,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
@@ -1366,7 +1366,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B45" t="inlineStr">
@@ -1387,7 +1387,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B46" t="inlineStr">
@@ -1408,7 +1408,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B47" t="inlineStr">
@@ -1429,7 +1429,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B48" t="inlineStr">
@@ -1450,7 +1450,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
@@ -1471,7 +1471,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
@@ -1492,7 +1492,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
@@ -1513,7 +1513,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
@@ -1534,7 +1534,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
@@ -1555,7 +1555,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
@@ -1576,7 +1576,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
@@ -1597,7 +1597,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
@@ -1618,7 +1618,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
@@ -1639,7 +1639,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
@@ -1660,7 +1660,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
@@ -1681,7 +1681,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
@@ -1702,7 +1702,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B61" t="inlineStr">
@@ -1723,7 +1723,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B62" t="inlineStr">
@@ -1744,7 +1744,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B63" t="inlineStr">
@@ -1765,7 +1765,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B64" t="inlineStr">
@@ -1786,7 +1786,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -1807,7 +1807,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -1828,7 +1828,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -1849,7 +1849,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B68" t="inlineStr">
@@ -1870,7 +1870,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B69" t="inlineStr">
@@ -1891,7 +1891,7 @@
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -1912,7 +1912,7 @@
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -1933,7 +1933,7 @@
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -1954,7 +1954,7 @@
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B73" t="inlineStr">
@@ -1975,7 +1975,7 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B74" t="inlineStr">
@@ -1996,7 +1996,7 @@
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B75" t="inlineStr">
@@ -2017,7 +2017,7 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B76" t="inlineStr">
@@ -2038,7 +2038,7 @@
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B77" t="inlineStr">
@@ -2059,7 +2059,7 @@
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B78" t="inlineStr">
@@ -2080,7 +2080,7 @@
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B79" t="inlineStr">
@@ -2101,7 +2101,7 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B80" t="inlineStr">
@@ -2122,7 +2122,7 @@
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B81" t="inlineStr">
@@ -2143,7 +2143,7 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B82" t="inlineStr">
@@ -2164,7 +2164,7 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B83" t="inlineStr">
@@ -2185,7 +2185,7 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B84" t="inlineStr">
@@ -2206,7 +2206,7 @@
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B85" t="inlineStr">
@@ -2227,7 +2227,7 @@
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B86" t="inlineStr">
@@ -2248,7 +2248,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B87" t="inlineStr">
@@ -2269,7 +2269,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B88" t="inlineStr">
@@ -2290,7 +2290,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B89" t="inlineStr">
@@ -2311,7 +2311,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B90" t="inlineStr">
@@ -2332,7 +2332,7 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B91" t="inlineStr">
@@ -2353,7 +2353,7 @@
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B92" t="inlineStr">
@@ -2374,7 +2374,7 @@
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B93" t="inlineStr">
@@ -2395,7 +2395,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B94" t="inlineStr">
@@ -2416,7 +2416,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B95" t="inlineStr">
@@ -2437,7 +2437,7 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B96" t="inlineStr">
@@ -2458,7 +2458,7 @@
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B97" t="inlineStr">
@@ -2479,7 +2479,7 @@
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B98" t="inlineStr">
@@ -2500,7 +2500,7 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B99" t="inlineStr">
@@ -2521,7 +2521,7 @@
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B100" t="inlineStr">
@@ -2542,7 +2542,7 @@
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B101" t="inlineStr">
@@ -2563,7 +2563,7 @@
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B102" t="inlineStr">
@@ -2584,7 +2584,7 @@
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B103" t="inlineStr">
@@ -2605,7 +2605,7 @@
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B104" t="inlineStr">
@@ -2626,7 +2626,7 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B105" t="inlineStr">
@@ -2647,7 +2647,7 @@
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B106" t="inlineStr">
@@ -2668,7 +2668,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B107" t="inlineStr">
@@ -2689,7 +2689,7 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B108" t="inlineStr">
@@ -2710,7 +2710,7 @@
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B109" t="inlineStr">
@@ -2731,7 +2731,7 @@
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B110" t="inlineStr">
@@ -2752,7 +2752,7 @@
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B111" t="inlineStr">
@@ -2773,7 +2773,7 @@
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B112" t="inlineStr">
@@ -2794,7 +2794,7 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B113" t="inlineStr">
@@ -2815,7 +2815,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B114" t="inlineStr">
@@ -2836,7 +2836,7 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B115" t="inlineStr">
@@ -2857,7 +2857,7 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B116" t="inlineStr">
@@ -2878,7 +2878,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B117" t="inlineStr">
@@ -2899,7 +2899,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -2920,7 +2920,7 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -2941,7 +2941,7 @@
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B120" t="inlineStr">
@@ -2962,7 +2962,7 @@
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B121" t="inlineStr">
@@ -2983,7 +2983,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3004,7 +3004,7 @@
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B123" t="inlineStr">
@@ -3025,7 +3025,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -3046,7 +3046,7 @@
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -3067,7 +3067,7 @@
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
@@ -3088,7 +3088,7 @@
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B127" t="inlineStr">
@@ -3109,7 +3109,7 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
@@ -3130,7 +3130,7 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
@@ -3151,7 +3151,7 @@
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -3172,7 +3172,7 @@
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
@@ -3193,7 +3193,7 @@
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
@@ -3214,7 +3214,7 @@
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
@@ -3235,7 +3235,7 @@
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
@@ -3256,7 +3256,7 @@
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
@@ -3277,7 +3277,7 @@
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B136" t="inlineStr">
@@ -3298,7 +3298,7 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
@@ -3319,7 +3319,7 @@
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
@@ -3340,7 +3340,7 @@
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
@@ -3361,7 +3361,7 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
@@ -3382,7 +3382,7 @@
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
@@ -3403,7 +3403,7 @@
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
@@ -3424,7 +3424,7 @@
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
@@ -3445,7 +3445,7 @@
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
@@ -3466,7 +3466,7 @@
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
@@ -3487,7 +3487,7 @@
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
@@ -3508,7 +3508,7 @@
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
@@ -3529,7 +3529,7 @@
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -3550,7 +3550,7 @@
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
@@ -3571,7 +3571,7 @@
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
@@ -3592,7 +3592,7 @@
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
@@ -3613,7 +3613,7 @@
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
@@ -3634,7 +3634,7 @@
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
@@ -3655,7 +3655,7 @@
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
@@ -3676,7 +3676,7 @@
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -3697,7 +3697,7 @@
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
@@ -3718,7 +3718,7 @@
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
@@ -3739,7 +3739,7 @@
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
@@ -3760,7 +3760,7 @@
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
@@ -3781,7 +3781,7 @@
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -3802,7 +3802,7 @@
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B161" t="inlineStr">
@@ -3823,7 +3823,7 @@
     <row r="162">
       <c r="A162" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B162" t="inlineStr">
@@ -3844,7 +3844,7 @@
     <row r="163">
       <c r="A163" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B163" t="inlineStr">
@@ -3865,7 +3865,7 @@
     <row r="164">
       <c r="A164" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B164" t="inlineStr">
@@ -3886,7 +3886,7 @@
     <row r="165">
       <c r="A165" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B165" t="inlineStr">
@@ -3907,7 +3907,7 @@
     <row r="166">
       <c r="A166" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B166" t="inlineStr">
@@ -3928,7 +3928,7 @@
     <row r="167">
       <c r="A167" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B167" t="inlineStr">
@@ -3949,7 +3949,7 @@
     <row r="168">
       <c r="A168" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B168" t="inlineStr">
@@ -3970,7 +3970,7 @@
     <row r="169">
       <c r="A169" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B169" t="inlineStr">
@@ -3991,7 +3991,7 @@
     <row r="170">
       <c r="A170" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B170" t="inlineStr">
@@ -4012,7 +4012,7 @@
     <row r="171">
       <c r="A171" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B171" t="inlineStr">
@@ -4033,7 +4033,7 @@
     <row r="172">
       <c r="A172" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B172" t="inlineStr">
@@ -4054,7 +4054,7 @@
     <row r="173">
       <c r="A173" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B173" t="inlineStr">
@@ -4075,7 +4075,7 @@
     <row r="174">
       <c r="A174" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B174" t="inlineStr">
@@ -4096,7 +4096,7 @@
     <row r="175">
       <c r="A175" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B175" t="inlineStr">
@@ -4117,7 +4117,7 @@
     <row r="176">
       <c r="A176" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B176" t="inlineStr">
@@ -4138,7 +4138,7 @@
     <row r="177">
       <c r="A177" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B177" t="inlineStr">
@@ -4159,7 +4159,7 @@
     <row r="178">
       <c r="A178" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B178" t="inlineStr">
@@ -4180,7 +4180,7 @@
     <row r="179">
       <c r="A179" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B179" t="inlineStr">
@@ -4201,7 +4201,7 @@
     <row r="180">
       <c r="A180" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B180" t="inlineStr">
@@ -4222,7 +4222,7 @@
     <row r="181">
       <c r="A181" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B181" t="inlineStr">
@@ -4243,7 +4243,7 @@
     <row r="182">
       <c r="A182" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B182" t="inlineStr">
@@ -4264,7 +4264,7 @@
     <row r="183">
       <c r="A183" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B183" t="inlineStr">
@@ -4285,7 +4285,7 @@
     <row r="184">
       <c r="A184" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B184" t="inlineStr">
@@ -4306,7 +4306,7 @@
     <row r="185">
       <c r="A185" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B185" t="inlineStr">
@@ -4327,7 +4327,7 @@
     <row r="186">
       <c r="A186" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B186" t="inlineStr">
@@ -4348,7 +4348,7 @@
     <row r="187">
       <c r="A187" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B187" t="inlineStr">
@@ -4369,7 +4369,7 @@
     <row r="188">
       <c r="A188" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B188" t="inlineStr">
@@ -4390,7 +4390,7 @@
     <row r="189">
       <c r="A189" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B189" t="inlineStr">
@@ -4411,7 +4411,7 @@
     <row r="190">
       <c r="A190" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B190" t="inlineStr">
@@ -4432,7 +4432,7 @@
     <row r="191">
       <c r="A191" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B191" t="inlineStr">
@@ -4453,7 +4453,7 @@
     <row r="192">
       <c r="A192" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B192" t="inlineStr">
@@ -4474,7 +4474,7 @@
     <row r="193">
       <c r="A193" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B193" t="inlineStr">
@@ -4495,7 +4495,7 @@
     <row r="194">
       <c r="A194" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B194" t="inlineStr">
@@ -4516,7 +4516,7 @@
     <row r="195">
       <c r="A195" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B195" t="inlineStr">
@@ -4537,7 +4537,7 @@
     <row r="196">
       <c r="A196" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B196" t="inlineStr">
@@ -4558,7 +4558,7 @@
     <row r="197">
       <c r="A197" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B197" t="inlineStr">
@@ -4579,7 +4579,7 @@
     <row r="198">
       <c r="A198" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B198" t="inlineStr">
@@ -4600,7 +4600,7 @@
     <row r="199">
       <c r="A199" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B199" t="inlineStr">
@@ -4621,7 +4621,7 @@
     <row r="200">
       <c r="A200" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B200" t="inlineStr">
@@ -4642,7 +4642,7 @@
     <row r="201">
       <c r="A201" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B201" t="inlineStr">
@@ -4663,7 +4663,7 @@
     <row r="202">
       <c r="A202" t="inlineStr">
         <is>
-          <t>CLINMISKIN GEL*</t>
+          <t>CLINMISKIN GEL</t>
         </is>
       </c>
       <c r="B202" t="inlineStr">

</xml_diff>